<commit_message>
best prediction updated with plots
</commit_message>
<xml_diff>
--- a/comparaison/ElasticNet.xlsx
+++ b/comparaison/ElasticNet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>alpha</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>0.07900677</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.08803612</t>
   </si>
 </sst>
 </file>
@@ -115,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -138,15 +144,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,6 +582,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>